<commit_message>
#19 - Exibicao de validacoes em tela
</commit_message>
<xml_diff>
--- a/documents/layouts_recadastramento/Layout_Retorno_Cadastro.xlsx
+++ b/documents/layouts_recadastramento/Layout_Retorno_Cadastro.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="657"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24600" windowHeight="15620" tabRatio="657" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="17" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="140">
   <si>
     <t>Nome do Campo</t>
   </si>
@@ -442,6 +442,9 @@
   </si>
   <si>
     <t>Entrevistado</t>
+  </si>
+  <si>
+    <t>Posição</t>
   </si>
 </sst>
 </file>
@@ -906,13 +909,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1326,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1337,117 +1335,117 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="24" thickBot="1">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>2</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="22">
         <v>3</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>3</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>3</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>2</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="40">
         <v>6</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="32"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>4</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>10</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="12"/>
+      <c r="E11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1462,657 +1460,857 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E59"/>
+  <dimension ref="B1:F56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="53" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="50" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="24" thickBot="1">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="2:6" ht="24" thickBot="1">
+      <c r="B1" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:6" ht="15" thickBot="1">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="10" t="s">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="38"/>
+      <c r="F3" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="2:6">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="5">
         <v>9</v>
       </c>
-      <c r="D4" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="10" t="s">
+      <c r="D4" s="5">
+        <f>SUM(C3,D3)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>25</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="5">
+        <f t="shared" ref="D5:D56" si="0">SUM(C4,D4)</f>
+        <v>12</v>
+      </c>
+      <c r="E5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="10" t="s">
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>1</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:6">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>1</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:6">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>1</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="12" t="s">
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="14" t="s">
+    <row r="9" spans="2:6">
+      <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>1</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="16" t="s">
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="48" t="s">
+    <row r="10" spans="2:6">
+      <c r="B10" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C10" s="46">
         <v>9</v>
       </c>
-      <c r="D11" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="51"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="10" t="s">
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="48"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C11" s="8">
         <v>50</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="10" t="s">
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="10" t="s">
+    <row r="13" spans="2:6">
+      <c r="B13" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C13" s="8">
         <v>14</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="10" t="s">
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C14" s="8">
         <v>9</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="10" t="s">
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C15" s="8">
         <v>2</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="10" t="s">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C16" s="8">
         <v>1</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="17" t="s">
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="10" t="s">
+    <row r="17" spans="2:6">
+      <c r="B17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C17" s="8">
         <v>10</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="10" t="s">
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C18" s="8">
         <v>10</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="10" t="s">
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C19" s="8">
         <v>30</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="1"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="48" t="s">
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C20" s="46">
         <v>9</v>
       </c>
-      <c r="D22" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="51"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="10" t="s">
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>177</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="48"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C21" s="8">
         <v>50</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="10" t="s">
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>186</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C22" s="8">
         <v>1</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="18" t="s">
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>236</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="10" t="s">
+    <row r="23" spans="2:6">
+      <c r="B23" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C23" s="8">
         <v>14</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="10" t="s">
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>237</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C24" s="8">
         <v>9</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="10" t="s">
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>251</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C25" s="8">
         <v>2</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="19"/>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="10" t="s">
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C26" s="8">
         <v>1</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="18" t="s">
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>262</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="10" t="s">
+    <row r="27" spans="2:6">
+      <c r="B27" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C27" s="8">
         <v>10</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="10" t="s">
+      <c r="D27" s="5">
+        <f t="shared" si="0"/>
+        <v>263</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C28" s="8">
         <v>10</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="10" t="s">
+      <c r="D28" s="5">
+        <f t="shared" si="0"/>
+        <v>273</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C29" s="8">
         <v>30</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="10" t="s">
+      <c r="D29" s="5">
+        <f t="shared" si="0"/>
+        <v>283</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C30" s="8">
         <v>2</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="10" t="s">
+      <c r="D30" s="5">
+        <f t="shared" si="0"/>
+        <v>313</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C31" s="8">
         <v>40</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="10" t="s">
+      <c r="D31" s="5">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C32" s="8">
         <v>5</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="10" t="s">
+      <c r="D32" s="5">
+        <f t="shared" si="0"/>
+        <v>355</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C33" s="8">
         <v>25</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="10" t="s">
+      <c r="D33" s="5">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C34" s="8">
         <v>20</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="10" t="s">
+      <c r="D34" s="5">
+        <f t="shared" si="0"/>
+        <v>385</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C35" s="8">
         <v>8</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="10" t="s">
+      <c r="D35" s="5">
+        <f t="shared" si="0"/>
+        <v>405</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C36" s="8">
         <v>15</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="1"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="48" t="s">
+      <c r="D36" s="5">
+        <f t="shared" si="0"/>
+        <v>413</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="C40" s="49">
+      <c r="C37" s="46">
         <v>9</v>
       </c>
-      <c r="D40" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="51"/>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="B41" s="10" t="s">
+      <c r="D37" s="5">
+        <f t="shared" si="0"/>
+        <v>428</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="48"/>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C38" s="8">
         <v>50</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12"/>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="10" t="s">
+      <c r="D38" s="5">
+        <f t="shared" si="0"/>
+        <v>437</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C39" s="8">
         <v>1</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="18" t="s">
+      <c r="D39" s="5">
+        <f t="shared" si="0"/>
+        <v>487</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
-      <c r="B43" s="10" t="s">
+    <row r="40" spans="2:6">
+      <c r="B40" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C40" s="8">
         <v>14</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="19"/>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="B44" s="10" t="s">
+      <c r="D40" s="5">
+        <f t="shared" si="0"/>
+        <v>488</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="16"/>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C41" s="8">
         <v>9</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="19"/>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="B45" s="10" t="s">
+      <c r="D41" s="5">
+        <f t="shared" si="0"/>
+        <v>502</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="16"/>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C42" s="8">
         <v>2</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D42" s="5">
+        <f t="shared" si="0"/>
+        <v>511</v>
+      </c>
+      <c r="E42" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="19"/>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="B46" s="10" t="s">
+      <c r="F42" s="16"/>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C43" s="8">
         <v>1</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="18" t="s">
+      <c r="D43" s="5">
+        <f t="shared" si="0"/>
+        <v>513</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
-      <c r="B47" s="10" t="s">
+    <row r="44" spans="2:6">
+      <c r="B44" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C44" s="8">
         <v>10</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="12"/>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="B48" s="10" t="s">
+      <c r="D44" s="5">
+        <f t="shared" si="0"/>
+        <v>514</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C45" s="8">
         <v>10</v>
       </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="12"/>
-    </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="10" t="s">
+      <c r="D45" s="5">
+        <f t="shared" si="0"/>
+        <v>524</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C46" s="8">
         <v>30</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="12"/>
-    </row>
-    <row r="50" spans="2:5">
-      <c r="B50" s="10" t="s">
+      <c r="D46" s="5">
+        <f t="shared" si="0"/>
+        <v>534</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C47" s="8">
         <v>2</v>
       </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="12"/>
-    </row>
-    <row r="51" spans="2:5">
-      <c r="B51" s="10" t="s">
+      <c r="D47" s="5">
+        <f t="shared" si="0"/>
+        <v>564</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C48" s="8">
         <v>40</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="12"/>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="B52" s="10" t="s">
+      <c r="D48" s="5">
+        <f t="shared" si="0"/>
+        <v>566</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C49" s="8">
         <v>5</v>
       </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="12"/>
-    </row>
-    <row r="53" spans="2:5">
-      <c r="B53" s="10" t="s">
+      <c r="D49" s="5">
+        <f t="shared" si="0"/>
+        <v>606</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C50" s="8">
         <v>25</v>
       </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="12"/>
-    </row>
-    <row r="54" spans="2:5">
-      <c r="B54" s="10" t="s">
+      <c r="D50" s="5">
+        <f t="shared" si="0"/>
+        <v>611</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C51" s="8">
         <v>20</v>
       </c>
-      <c r="D54" s="11"/>
-      <c r="E54" s="12"/>
-    </row>
-    <row r="55" spans="2:5">
-      <c r="B55" s="10" t="s">
+      <c r="D51" s="5">
+        <f t="shared" si="0"/>
+        <v>636</v>
+      </c>
+      <c r="E51" s="8"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C52" s="8">
         <v>8</v>
       </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="12"/>
-    </row>
-    <row r="56" spans="2:5" ht="15" thickBot="1">
-      <c r="B56" s="20" t="s">
+      <c r="D52" s="5">
+        <f t="shared" si="0"/>
+        <v>656</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="2:6" ht="15" thickBot="1">
+      <c r="B53" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="21">
+      <c r="C53" s="18">
         <v>15</v>
       </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="23"/>
-    </row>
-    <row r="57" spans="2:5">
-      <c r="B57" s="10" t="s">
+      <c r="D53" s="5">
+        <f t="shared" si="0"/>
+        <v>664</v>
+      </c>
+      <c r="E53" s="18"/>
+      <c r="F53" s="20"/>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C54" s="8">
         <v>20</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="D54" s="5">
+        <f t="shared" si="0"/>
+        <v>679</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="12"/>
-    </row>
-    <row r="58" spans="2:5" ht="15" thickBot="1">
-      <c r="B58" s="20" t="s">
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="2:6" ht="15" thickBot="1">
+      <c r="B55" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C58" s="21">
+      <c r="C55" s="18">
         <v>20</v>
       </c>
-      <c r="D58" s="21" t="s">
+      <c r="D55" s="5">
+        <f t="shared" si="0"/>
+        <v>699</v>
+      </c>
+      <c r="E55" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E58" s="23"/>
-    </row>
-    <row r="59" spans="2:5">
-      <c r="B59" s="34" t="s">
+      <c r="F55" s="20"/>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="36">
+      <c r="C56" s="33">
         <v>26</v>
       </c>
-      <c r="D59" s="47" t="s">
+      <c r="D56" s="5">
+        <f t="shared" si="0"/>
+        <v>719</v>
+      </c>
+      <c r="E56" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="E59" s="35"/>
+      <c r="F56" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2127,544 +2325,672 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G46"/>
+  <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="53"/>
-    <col min="5" max="5" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="50"/>
+    <col min="6" max="6" width="50.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="24" thickBot="1">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="2:6" ht="24" thickBot="1">
+      <c r="B1" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:6" ht="15" thickBot="1">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="10" t="s">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="2:6" ht="15" thickBot="1">
+      <c r="B3" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="38"/>
+      <c r="F3" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="24" t="s">
+    <row r="4" spans="2:6">
+      <c r="B4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="22">
         <v>9</v>
       </c>
-      <c r="D4" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="26"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="37" t="s">
+      <c r="D4" s="5">
+        <f>SUM(C3,D3)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="35">
         <v>30</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="39"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="10" t="s">
+      <c r="D5" s="5">
+        <f t="shared" ref="D5:D41" si="0">SUM(C4,D4)</f>
+        <v>12</v>
+      </c>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>17</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:6">
+      <c r="B7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>2</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="10" t="s">
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>2</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="40" t="s">
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="38">
         <v>8</v>
       </c>
-      <c r="D9" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="10" t="s">
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>31</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="10" t="s">
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>20</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="10" t="s">
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>5</v>
       </c>
-      <c r="D12" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="10" t="s">
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="8">
         <v>5</v>
       </c>
-      <c r="D13" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="10" t="s">
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C14" s="8">
         <v>2</v>
       </c>
-      <c r="D15" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="10" t="s">
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C15" s="8">
         <v>40</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="10" t="s">
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C16" s="8">
         <v>5</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="10" t="s">
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C17" s="8">
         <v>25</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="10" t="s">
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C18" s="8">
         <v>20</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="10" t="s">
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C19" s="8">
         <v>8</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="10" t="s">
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>224</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C20" s="8">
         <v>15</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="10" t="s">
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>232</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C21" s="8">
         <v>9</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="1"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="10" t="s">
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C22" s="8">
         <v>3</v>
       </c>
-      <c r="D24" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="12" t="s">
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="10" t="s">
+    <row r="23" spans="2:6">
+      <c r="B23" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C23" s="8">
         <v>3</v>
       </c>
-      <c r="D25" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="12" t="s">
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>259</v>
+      </c>
+      <c r="E23" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="10" t="s">
+    <row r="24" spans="2:6">
+      <c r="B24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C24" s="8">
         <v>3</v>
       </c>
-      <c r="D26" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="12" t="s">
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>262</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="10" t="s">
+    <row r="25" spans="2:6">
+      <c r="B25" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C25" s="8">
         <v>3</v>
       </c>
-      <c r="D27" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="12" t="s">
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
+        <v>265</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="1"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="10" t="s">
+    <row r="26" spans="2:6">
+      <c r="B26" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C26" s="8">
         <v>3</v>
       </c>
-      <c r="D29" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="12" t="s">
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>268</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="10" t="s">
+    <row r="27" spans="2:6">
+      <c r="B27" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C27" s="8">
         <v>3</v>
       </c>
-      <c r="D30" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="12" t="s">
+      <c r="D27" s="5">
+        <f t="shared" si="0"/>
+        <v>271</v>
+      </c>
+      <c r="E27" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="10" t="s">
+    <row r="28" spans="2:6">
+      <c r="B28" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C28" s="8">
         <v>3</v>
       </c>
-      <c r="D31" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="12" t="s">
+      <c r="D28" s="5">
+        <f t="shared" si="0"/>
+        <v>274</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="10" t="s">
+    <row r="29" spans="2:6">
+      <c r="B29" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C29" s="8">
         <v>3</v>
       </c>
-      <c r="D32" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="12" t="s">
+      <c r="D29" s="5">
+        <f t="shared" si="0"/>
+        <v>277</v>
+      </c>
+      <c r="E29" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
-      <c r="B33" s="1"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="10" t="s">
+    <row r="30" spans="2:6">
+      <c r="B30" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C30" s="8">
         <v>3</v>
       </c>
-      <c r="D34" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="12" t="s">
+      <c r="D30" s="5">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
-      <c r="B35" s="10" t="s">
+    <row r="31" spans="2:6">
+      <c r="B31" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C31" s="8">
         <v>3</v>
       </c>
-      <c r="D35" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="12" t="s">
+      <c r="D31" s="5">
+        <f t="shared" si="0"/>
+        <v>283</v>
+      </c>
+      <c r="E31" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
-      <c r="B36" s="10" t="s">
+    <row r="32" spans="2:6">
+      <c r="B32" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C32" s="8">
         <v>3</v>
       </c>
-      <c r="D36" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="12" t="s">
+      <c r="D32" s="5">
+        <f t="shared" si="0"/>
+        <v>286</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="2:7">
-      <c r="B37" s="10" t="s">
+    <row r="33" spans="2:8">
+      <c r="B33" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C33" s="8">
         <v>3</v>
       </c>
-      <c r="D37" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="12" t="s">
+      <c r="D33" s="5">
+        <f t="shared" si="0"/>
+        <v>289</v>
+      </c>
+      <c r="E33" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
-      <c r="B38" s="1"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="2:7">
-      <c r="B39" s="10" t="s">
+    <row r="34" spans="2:8">
+      <c r="B34" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C34" s="8">
         <v>3</v>
       </c>
-      <c r="D39" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="12" t="s">
+      <c r="D34" s="5">
+        <f t="shared" si="0"/>
+        <v>292</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="2:7">
-      <c r="B40" s="10" t="s">
+    <row r="35" spans="2:8">
+      <c r="B35" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C35" s="8">
         <v>3</v>
       </c>
-      <c r="D40" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="12" t="s">
+      <c r="D35" s="5">
+        <f t="shared" si="0"/>
+        <v>295</v>
+      </c>
+      <c r="E35" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="2:7">
-      <c r="B41" s="10" t="s">
+    <row r="36" spans="2:8">
+      <c r="B36" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C36" s="8">
         <v>3</v>
       </c>
-      <c r="D41" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="12" t="s">
+      <c r="D36" s="5">
+        <f t="shared" si="0"/>
+        <v>298</v>
+      </c>
+      <c r="E36" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="2:7">
-      <c r="B42" s="10" t="s">
+    <row r="37" spans="2:8">
+      <c r="B37" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C37" s="8">
         <v>3</v>
       </c>
-      <c r="D42" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="12" t="s">
+      <c r="D37" s="5">
+        <f t="shared" si="0"/>
+        <v>301</v>
+      </c>
+      <c r="E37" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="2:7">
-      <c r="B43" s="10" t="s">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="41">
+      <c r="C38" s="38">
         <v>2</v>
       </c>
-      <c r="D43" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="17" t="s">
+      <c r="D38" s="5">
+        <f t="shared" si="0"/>
+        <v>304</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:7">
-      <c r="B44" s="10" t="s">
+    <row r="39" spans="2:8">
+      <c r="B39" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C39" s="8">
         <v>20</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D39" s="5">
+        <f t="shared" si="0"/>
+        <v>306</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="2:7" ht="15" thickBot="1">
-      <c r="B45" s="20" t="s">
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="2:8" ht="15" thickBot="1">
+      <c r="B40" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="21">
+      <c r="C40" s="18">
         <v>20</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D40" s="5">
+        <f t="shared" si="0"/>
+        <v>326</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="23"/>
-    </row>
-    <row r="46" spans="2:7">
-      <c r="B46" s="34" t="s">
+      <c r="F40" s="20"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="36">
+      <c r="C41" s="33">
         <v>26</v>
       </c>
-      <c r="D46" s="47" t="s">
+      <c r="D41" s="5">
+        <f t="shared" si="0"/>
+        <v>346</v>
+      </c>
+      <c r="E41" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="E46" s="35"/>
+      <c r="F41" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2694,55 +3020,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="24" thickBot="1">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="22">
         <v>9</v>
       </c>
-      <c r="D4" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="28"/>
+      <c r="D4" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>3</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2769,124 +3095,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="24" thickBot="1">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="15" thickBot="1">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
         <v>9</v>
       </c>
-      <c r="D4" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="17"/>
+      <c r="D4" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="38">
         <v>2</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="30" t="s">
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="38">
         <v>2</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="30" t="s">
+      <c r="D6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="38">
         <v>2</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="33" t="s">
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="30" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>20</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:7" ht="15" thickBot="1">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>20</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="G9" s="5"/>
+      <c r="E9" s="20"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="33">
         <v>26</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="35"/>
+      <c r="E10" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2915,145 +3241,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="24" thickBot="1">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="15" thickBot="1">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="42">
         <v>2</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46" t="s">
+      <c r="D3" s="42"/>
+      <c r="E3" s="43" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="42">
         <v>9</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="46"/>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>10</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>2</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="12"/>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>2</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="40">
         <v>2</v>
       </c>
-      <c r="D9" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="32" t="s">
+      <c r="D9" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>20</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>20</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>26</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3081,141 +3407,141 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="24" thickBot="1">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="15" thickBot="1">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" ht="15" thickBot="1">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="42">
         <v>2</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46" t="s">
+      <c r="D4" s="42"/>
+      <c r="E4" s="43" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="22">
         <v>9</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="28"/>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
         <v>3</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="12"/>
+      <c r="D6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
         <v>200</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
         <v>30</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
         <v>30</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
         <v>20</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <v>20</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
         <v>26</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="46">
         <v>20</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="50"/>
+      <c r="E13" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>